<commit_message>
fix(recognition): confirmation grid, employee parser prefers metricCol, centralize uploads pointer in Step1
</commit_message>
<xml_diff>
--- a/PocketManager5_sitetmpupload_samples/EPR sample file.xlsx
+++ b/PocketManager5_sitetmpupload_samples/EPR sample file.xlsx
@@ -3023,7 +3023,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3033,9 +3033,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:X478"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:24">
       <c r="A1" t="s">

</xml_diff>